<commit_message>
app update and new tiering.xlsx
</commit_message>
<xml_diff>
--- a/survey_shiny/bb4FAIR_app/tiering.xlsx
+++ b/survey_shiny/bb4FAIR_app/tiering.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/federica/Documents/GitHub/BB4FAIR/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\BB4FAIR-main\BB4FAIR-main\survey_shiny\bb4FAIR_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D108BDAF-2646-AD48-9B63-F404EF9C088F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1CD43E-E2B6-4CD3-AD96-82E183C15100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="-21600" windowWidth="19000" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="total_score" sheetId="1" r:id="rId1"/>
+    <sheet name="punteggi_totali" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">punteggi_totali!$B$1:$P$38</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +37,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Biobank name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+  <si>
+    <t>Biobank ID</t>
+  </si>
+  <si>
+    <t>BIMS</t>
+  </si>
+  <si>
+    <t>annotations</t>
+  </si>
+  <si>
+    <t>total_score</t>
+  </si>
+  <si>
+    <t>Centro Risorse Biologiche (CRB)</t>
+  </si>
+  <si>
+    <t>Biobanca di Ricerca OPBG</t>
+  </si>
+  <si>
+    <t>CRB IRST</t>
+  </si>
+  <si>
+    <t>IRCCS ISTITUTO NAZIONALE TUMORI REGINA ELENA  BBIRE</t>
+  </si>
+  <si>
+    <t>Biobanca Cardiovascolare BioCor</t>
+  </si>
+  <si>
+    <t>Centro Risiorse Biologiche Istituto Ortopedico Rizzoli - CRB IOR</t>
+  </si>
+  <si>
+    <t>Biobanca di ricerca AUSL - IRCCS di Reggio Emilia</t>
+  </si>
+  <si>
+    <t>Biobanca Istituzionale BBI</t>
+  </si>
+  <si>
+    <t>Tropica Biobank</t>
+  </si>
+  <si>
+    <t>UPO Biobank</t>
+  </si>
+  <si>
+    <t>Biobanca di ricerca per la medicina personalizzata</t>
+  </si>
+  <si>
+    <t>Biobanca Bruno Boerci di ICS Maugeri</t>
+  </si>
+  <si>
+    <t>BioBanca Istituzionale Bari</t>
+  </si>
+  <si>
+    <t>Humanitas Hospital Biological Resource Center</t>
+  </si>
+  <si>
+    <t>BIOGER - Biobanca Istituzionale dell'IRCCS INRCA, Ancona</t>
+  </si>
+  <si>
+    <t>CCPP Biobank</t>
+  </si>
+  <si>
+    <t>Centro Raccolta Materiale Biologico Alessandria Biobank</t>
+  </si>
+  <si>
+    <t>CHRIS Biobank</t>
+  </si>
+  <si>
+    <t>ARC-Net</t>
+  </si>
+  <si>
+    <t>Biobank of Veterinary Resources</t>
+  </si>
+  <si>
+    <t>Banca Biologica INMI L Spallanzani (bbmri-eric:ID:IT_1384262955037988)</t>
+  </si>
+  <si>
+    <t>SATURNE</t>
+  </si>
+  <si>
+    <t>Biobanca del Laboratorio di Genetica Umana</t>
+  </si>
+  <si>
+    <t>Biobanca del CRESM, CRESM Biobank</t>
+  </si>
+  <si>
+    <t>Biobanca IRCCS Istituto Centro San Giovanni di Dio Fatebenefratelli (Biobank FBF)</t>
+  </si>
+  <si>
+    <t>Centro Risorse Biologiche/Biobanca POLI-MI</t>
+  </si>
+  <si>
+    <t>SSD BIOBANCA ASST PAPA GIOVANNI XXIII BERGAMO</t>
+  </si>
+  <si>
+    <t>CRB Centro Risorse Biologiche Neurome Biobanking Center</t>
+  </si>
+  <si>
+    <t>BCU Imaging Biobank</t>
+  </si>
+  <si>
+    <t>Genetic Biobank of Siena</t>
+  </si>
+  <si>
+    <t>Banca Tessuti Tumorali Chirurgia Generale 3</t>
+  </si>
+  <si>
+    <t>da Vinci European BioBank - daVEB</t>
+  </si>
+  <si>
+    <t>Neuromuscular Bank of Tissues and DNA samples</t>
+  </si>
+  <si>
+    <t>Neuromuscular Disease Biobank</t>
+  </si>
+  <si>
+    <t>Banca Biologica Oncologica Pediatrica</t>
+  </si>
+  <si>
+    <t>LRPO-ISPRO</t>
+  </si>
+  <si>
+    <t>Biobanca - INT Milano</t>
+  </si>
+  <si>
+    <t>Biobank_name</t>
   </si>
   <si>
     <t>IT_head</t>
@@ -50,56 +174,41 @@
     <t>ontologies_richness</t>
   </si>
   <si>
-    <t>common_data_model</t>
-  </si>
-  <si>
-    <t>BIMS</t>
+    <t>common_data_models</t>
   </si>
   <si>
     <t>data_management</t>
   </si>
   <si>
-    <t>IT_infrastructures</t>
-  </si>
-  <si>
     <t>massive_storage</t>
   </si>
   <si>
-    <t>IT_components</t>
-  </si>
-  <si>
     <t>data_warehouse</t>
   </si>
   <si>
     <t>clinical_data_availability</t>
   </si>
   <si>
-    <t>annotations</t>
-  </si>
-  <si>
     <t>registry_data_availability</t>
   </si>
   <si>
     <t>informed_consent</t>
   </si>
   <si>
-    <t>total_score</t>
+    <t>data_server</t>
+  </si>
+  <si>
+    <t>service_resources</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,9 +234,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -426,66 +534,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -496,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -520,7 +643,7 @@
         <v>2</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -532,10 +655,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -546,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -564,28 +687,28 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -596,46 +719,46 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -646,7 +769,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -661,16 +784,16 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>2</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -682,15 +805,15 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -702,19 +825,19 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -723,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -732,10 +855,10 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -764,16 +887,16 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -782,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -796,10 +919,10 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>8</v>
@@ -811,57 +934,57 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>2</v>
@@ -882,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -893,19 +1016,19 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>2</v>
@@ -917,25 +1040,25 @@
         <v>2</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>3</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
       <c r="P10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -943,49 +1066,49 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <v>2</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -993,16 +1116,16 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1017,89 +1140,89 @@
         <v>2</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N12">
         <v>1</v>
       </c>
       <c r="O12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>3</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1120,10 +1243,10 @@
         <v>2</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1132,27 +1255,27 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1161,16 +1284,16 @@
         <v>2</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -1185,7 +1308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1193,28 +1316,28 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>2</v>
@@ -1226,51 +1349,51 @@
         <v>3</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
         <v>3</v>
@@ -1282,10 +1405,10 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1293,31 +1416,31 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1332,10 +1455,10 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1343,49 +1466,49 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1399,7 +1522,7 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1408,19 +1531,19 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>3</v>
@@ -1432,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1446,13 +1569,13 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1464,10 +1587,10 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1476,17 +1599,17 @@
         <v>3</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
@@ -1496,7 +1619,7 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1508,22 +1631,22 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -1532,21 +1655,21 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1558,13 +1681,13 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1576,16 +1699,16 @@
         <v>3</v>
       </c>
       <c r="N23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
       <c r="P23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1593,19 +1716,19 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <v>2</v>
@@ -1617,25 +1740,25 @@
         <v>2</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24">
         <v>3</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1646,16 +1769,16 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1682,27 +1805,27 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1711,10 +1834,10 @@
         <v>2</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1723,19 +1846,19 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1746,7 +1869,7 @@
         <v>4</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1761,10 +1884,10 @@
         <v>2</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -1776,30 +1899,30 @@
         <v>3</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1814,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1832,27 +1955,27 @@
         <v>0</v>
       </c>
       <c r="P28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1861,31 +1984,31 @@
         <v>2</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
       <c r="P29">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1896,13 +2019,13 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1911,31 +2034,31 @@
         <v>2</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L30">
         <v>0</v>
       </c>
       <c r="M30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1943,19 +2066,19 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>2</v>
@@ -1976,16 +2099,16 @@
         <v>2</v>
       </c>
       <c r="N31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1996,7 +2119,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2011,10 +2134,10 @@
         <v>2</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2023,19 +2146,19 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
       <c r="P32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2046,22 +2169,22 @@
         <v>4</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -2076,24 +2199,24 @@
         <v>3</v>
       </c>
       <c r="N33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
       <c r="P33">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -2102,13 +2225,13 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -2117,7 +2240,7 @@
         <v>2</v>
       </c>
       <c r="K34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L34">
         <v>0</v>
@@ -2126,16 +2249,16 @@
         <v>3</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="P34">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2143,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2152,10 +2275,10 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -2164,7 +2287,7 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2182,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="P35">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2196,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -2211,10 +2334,10 @@
         <v>2</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -2223,7 +2346,7 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -2232,21 +2355,21 @@
         <v>0</v>
       </c>
       <c r="P36">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2273,7 +2396,7 @@
         <v>0</v>
       </c>
       <c r="M37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N37">
         <v>1</v>
@@ -2285,7 +2408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2293,10 +2416,10 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2308,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -2332,15 +2455,450 @@
         <v>0</v>
       </c>
       <c r="P38">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P48">
-    <sortCondition ref="A1:A48"/>
-  </sortState>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <autoFilter ref="A1:P38" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDD1576-19EA-4DEA-B3FA-A1D1C0C0B841}">
+  <dimension ref="A1:C38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>